<commit_message>
update test run hms
</commit_message>
<xml_diff>
--- a/data/demo/hujan_kasus1 - Copy.xlsx
+++ b/data/demo/hujan_kasus1 - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\62812\Documents\Kerjaan Meteorologi\FEWS BNPB\Code\github\EWS of Flood Forecast\notebooks\Data Preparation Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\62812\Documents\Kerjaan Meteorologi\FEWS BNPB\hms_deployment\hms_deployment\data\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7F0FBB-E0AA-470F-9730-DFE1ED139C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F05AEBF-D5E2-4732-86F4-5DDAC700D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A1E0B86-2AC2-462D-8837-DF22D256CCA9}"/>
   </bookViews>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB40C62-8513-441D-B841-62E26F78FF49}">
   <dimension ref="A1:F721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="K339" sqref="K339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,13 +531,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -551,13 +551,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -571,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -591,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -611,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -631,13 +631,13 @@
         <v>1.5</v>
       </c>
       <c r="D8" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -651,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -671,13 +671,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -691,13 +691,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -711,13 +711,13 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -731,13 +731,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -751,13 +751,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -771,13 +771,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,13 +811,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -831,13 +831,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -851,13 +851,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,13 +871,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F20" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,13 +891,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -911,13 +911,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -931,13 +931,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -951,13 +951,13 @@
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,13 +971,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -991,13 +991,13 @@
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1011,13 +1011,13 @@
         <v>2</v>
       </c>
       <c r="D27" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E27" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F27" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1031,13 +1031,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F28" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1051,13 +1051,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1071,13 +1071,13 @@
         <v>0</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1091,13 +1091,13 @@
         <v>0.5</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1111,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F32" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1131,13 +1131,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1151,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F34" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1171,13 +1171,13 @@
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F35" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,13 +1191,13 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F36" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1211,13 +1211,13 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1231,13 +1231,13 @@
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E38" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F38" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1251,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="D39" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F39" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1271,13 +1271,13 @@
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2291,13 +2291,13 @@
         <v>0</v>
       </c>
       <c r="D91" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E91" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F91" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2311,13 +2311,13 @@
         <v>0</v>
       </c>
       <c r="D92" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E92" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F92" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2331,13 +2331,13 @@
         <v>0</v>
       </c>
       <c r="D93" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E93" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F93" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2351,13 +2351,13 @@
         <v>0</v>
       </c>
       <c r="D94" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E94" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F94" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2371,13 +2371,13 @@
         <v>0</v>
       </c>
       <c r="D95" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E95" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F95" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2391,13 +2391,13 @@
         <v>0</v>
       </c>
       <c r="D96" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E96" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F96" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2411,13 +2411,13 @@
         <v>0</v>
       </c>
       <c r="D97" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E97" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F97" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2431,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="D98" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E98" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F98" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2451,13 +2451,13 @@
         <v>0</v>
       </c>
       <c r="D99" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E99" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F99" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2471,13 +2471,13 @@
         <v>0</v>
       </c>
       <c r="D100" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E100" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F100" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2491,13 +2491,13 @@
         <v>0</v>
       </c>
       <c r="D101" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E101" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F101" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2511,13 +2511,13 @@
         <v>0</v>
       </c>
       <c r="D102" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E102" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F102" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,13 +2531,13 @@
         <v>0</v>
       </c>
       <c r="D103" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E103" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F103" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2551,13 +2551,13 @@
         <v>0</v>
       </c>
       <c r="D104" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E104" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F104" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2571,13 +2571,13 @@
         <v>0.5</v>
       </c>
       <c r="D105" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E105" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F105" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,13 +2591,13 @@
         <v>0</v>
       </c>
       <c r="D106" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E106" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F106" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2611,13 +2611,13 @@
         <v>0</v>
       </c>
       <c r="D107" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E107" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F107" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="D108" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E108" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F108" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2651,13 +2651,13 @@
         <v>0</v>
       </c>
       <c r="D109" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E109" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F109" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2671,13 +2671,13 @@
         <v>0</v>
       </c>
       <c r="D110" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E110" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F110" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,13 +2691,13 @@
         <v>0</v>
       </c>
       <c r="D111" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E111" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F111" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2711,13 +2711,13 @@
         <v>0</v>
       </c>
       <c r="D112" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E112" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F112" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -2731,13 +2731,13 @@
         <v>0</v>
       </c>
       <c r="D113" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E113" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F113" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="D114" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E114" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F114" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -2771,13 +2771,13 @@
         <v>0</v>
       </c>
       <c r="D115" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E115" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F115" s="3">
-        <v>22.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -2791,13 +2791,13 @@
         <v>0</v>
       </c>
       <c r="D116" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E116" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F116" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -2811,13 +2811,13 @@
         <v>0</v>
       </c>
       <c r="D117" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E117" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F117" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -2831,13 +2831,13 @@
         <v>0</v>
       </c>
       <c r="D118" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E118" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F118" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -2851,13 +2851,13 @@
         <v>0</v>
       </c>
       <c r="D119" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E119" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F119" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -2871,13 +2871,13 @@
         <v>0</v>
       </c>
       <c r="D120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -2891,13 +2891,13 @@
         <v>0</v>
       </c>
       <c r="D121" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E121" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F121" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -2911,13 +2911,13 @@
         <v>0</v>
       </c>
       <c r="D122" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E122" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F122" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,13 +2931,13 @@
         <v>0</v>
       </c>
       <c r="D123" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E123" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F123" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -2951,13 +2951,13 @@
         <v>0</v>
       </c>
       <c r="D124" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E124" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F124" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -2971,13 +2971,13 @@
         <v>0</v>
       </c>
       <c r="D125" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E125" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F125" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -2991,13 +2991,13 @@
         <v>0</v>
       </c>
       <c r="D126" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E126" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F126" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3011,13 +3011,13 @@
         <v>0</v>
       </c>
       <c r="D127" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E127" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F127" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3031,13 +3031,13 @@
         <v>0</v>
       </c>
       <c r="D128" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E128" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F128" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -6631,13 +6631,13 @@
         <v>0</v>
       </c>
       <c r="D308" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E308" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F308" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
@@ -6651,13 +6651,13 @@
         <v>0</v>
       </c>
       <c r="D309" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E309" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F309" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
@@ -6671,13 +6671,13 @@
         <v>0</v>
       </c>
       <c r="D310" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E310" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F310" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.3">
@@ -6691,13 +6691,13 @@
         <v>0</v>
       </c>
       <c r="D311" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E311" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F311" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.3">
@@ -6711,13 +6711,13 @@
         <v>0</v>
       </c>
       <c r="D312" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E312" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F312" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.3">
@@ -6731,13 +6731,13 @@
         <v>0</v>
       </c>
       <c r="D313" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E313" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F313" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
@@ -6751,13 +6751,13 @@
         <v>0</v>
       </c>
       <c r="D314" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E314" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F314" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
@@ -6771,13 +6771,13 @@
         <v>0</v>
       </c>
       <c r="D315" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E315" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F315" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
@@ -6791,13 +6791,13 @@
         <v>0</v>
       </c>
       <c r="D316" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E316" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F316" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
@@ -6811,13 +6811,13 @@
         <v>0</v>
       </c>
       <c r="D317" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E317" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F317" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
@@ -6831,13 +6831,13 @@
         <v>0</v>
       </c>
       <c r="D318" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E318" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F318" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.3">
@@ -6851,13 +6851,13 @@
         <v>0</v>
       </c>
       <c r="D319" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E319" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F319" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.3">
@@ -6871,13 +6871,13 @@
         <v>0</v>
       </c>
       <c r="D320" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E320" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F320" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.3">
@@ -6891,13 +6891,13 @@
         <v>0</v>
       </c>
       <c r="D321" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E321" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F321" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.3">
@@ -6911,13 +6911,13 @@
         <v>0</v>
       </c>
       <c r="D322" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E322" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F322" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
@@ -6931,13 +6931,13 @@
         <v>0</v>
       </c>
       <c r="D323" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E323" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F323" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.3">
@@ -6951,13 +6951,13 @@
         <v>0</v>
       </c>
       <c r="D324" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E324" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F324" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.3">
@@ -6971,13 +6971,13 @@
         <v>0</v>
       </c>
       <c r="D325" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E325" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F325" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.3">
@@ -6991,13 +6991,13 @@
         <v>0</v>
       </c>
       <c r="D326" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E326" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F326" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
@@ -7011,13 +7011,13 @@
         <v>0</v>
       </c>
       <c r="D327" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E327" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F327" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.3">
@@ -7031,13 +7031,13 @@
         <v>0</v>
       </c>
       <c r="D328" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E328" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F328" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.3">
@@ -7051,13 +7051,13 @@
         <v>0</v>
       </c>
       <c r="D329" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E329" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F329" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
@@ -7071,13 +7071,13 @@
         <v>0</v>
       </c>
       <c r="D330" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E330" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F330" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
@@ -7091,13 +7091,13 @@
         <v>2.5</v>
       </c>
       <c r="D331" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E331" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F331" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.3">
@@ -7111,13 +7111,13 @@
         <v>0</v>
       </c>
       <c r="D332" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E332" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F332" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.3">
@@ -7131,13 +7131,13 @@
         <v>0</v>
       </c>
       <c r="D333" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E333" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F333" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
@@ -7151,13 +7151,13 @@
         <v>0</v>
       </c>
       <c r="D334" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E334" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F334" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
@@ -7171,13 +7171,13 @@
         <v>0</v>
       </c>
       <c r="D335" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E335" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F335" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
@@ -7191,13 +7191,13 @@
         <v>0</v>
       </c>
       <c r="D336" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E336" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F336" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
@@ -7211,13 +7211,13 @@
         <v>0</v>
       </c>
       <c r="D337" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E337" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F337" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
@@ -7231,13 +7231,13 @@
         <v>0</v>
       </c>
       <c r="D338" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E338" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F338" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.3">
@@ -7251,13 +7251,13 @@
         <v>0</v>
       </c>
       <c r="D339" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E339" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F339" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.3">
@@ -7271,13 +7271,13 @@
         <v>0</v>
       </c>
       <c r="D340" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E340" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F340" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.3">
@@ -7291,13 +7291,13 @@
         <v>0</v>
       </c>
       <c r="D341" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E341" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F341" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
@@ -7311,13 +7311,13 @@
         <v>0</v>
       </c>
       <c r="D342" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E342" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F342" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
@@ -7331,13 +7331,13 @@
         <v>0</v>
       </c>
       <c r="D343" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E343" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F343" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.3">
@@ -7351,13 +7351,13 @@
         <v>0</v>
       </c>
       <c r="D344" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E344" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F344" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.3">
@@ -7371,13 +7371,13 @@
         <v>0</v>
       </c>
       <c r="D345" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E345" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F345" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
@@ -8911,13 +8911,13 @@
         <v>0</v>
       </c>
       <c r="D422" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E422" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F422" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.3">
@@ -8931,13 +8931,13 @@
         <v>0</v>
       </c>
       <c r="D423" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E423" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F423" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="424" spans="1:6" x14ac:dyDescent="0.3">
@@ -8951,13 +8951,13 @@
         <v>0</v>
       </c>
       <c r="D424" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E424" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F424" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="425" spans="1:6" x14ac:dyDescent="0.3">
@@ -8971,13 +8971,13 @@
         <v>0</v>
       </c>
       <c r="D425" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E425" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F425" s="3">
-        <v>11.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="426" spans="1:6" x14ac:dyDescent="0.3">
@@ -8991,13 +8991,13 @@
         <v>0</v>
       </c>
       <c r="D426" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E426" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F426" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.3">
@@ -9011,13 +9011,13 @@
         <v>0</v>
       </c>
       <c r="D427" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E427" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F427" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.3">
@@ -9031,13 +9031,13 @@
         <v>0</v>
       </c>
       <c r="D428" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E428" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F428" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.3">
@@ -9051,13 +9051,13 @@
         <v>0</v>
       </c>
       <c r="D429" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E429" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F429" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.3">
@@ -9071,13 +9071,13 @@
         <v>0.5</v>
       </c>
       <c r="D430" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E430" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F430" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.3">
@@ -9091,13 +9091,13 @@
         <v>0.5</v>
       </c>
       <c r="D431" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E431" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F431" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.3">
@@ -9111,13 +9111,13 @@
         <v>0.5</v>
       </c>
       <c r="D432" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E432" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F432" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.3">
@@ -9131,13 +9131,13 @@
         <v>1</v>
       </c>
       <c r="D433" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E433" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F433" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.3">
@@ -9151,13 +9151,13 @@
         <v>0</v>
       </c>
       <c r="D434" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E434" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F434" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.3">
@@ -9171,13 +9171,13 @@
         <v>0</v>
       </c>
       <c r="D435" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E435" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F435" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.3">
@@ -9191,13 +9191,13 @@
         <v>0</v>
       </c>
       <c r="D436" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E436" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F436" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="437" spans="1:6" x14ac:dyDescent="0.3">
@@ -9211,13 +9211,13 @@
         <v>0</v>
       </c>
       <c r="D437" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E437" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F437" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.3">
@@ -9231,13 +9231,13 @@
         <v>0</v>
       </c>
       <c r="D438" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E438" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F438" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.3">
@@ -9251,13 +9251,13 @@
         <v>0</v>
       </c>
       <c r="D439" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E439" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F439" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.3">
@@ -9271,13 +9271,13 @@
         <v>0</v>
       </c>
       <c r="D440" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E440" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F440" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.3">
@@ -9291,13 +9291,13 @@
         <v>0</v>
       </c>
       <c r="D441" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E441" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F441" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.3">
@@ -9311,13 +9311,13 @@
         <v>0</v>
       </c>
       <c r="D442" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E442" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F442" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.3">
@@ -9331,13 +9331,13 @@
         <v>0</v>
       </c>
       <c r="D443" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E443" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F443" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.3">
@@ -9351,13 +9351,13 @@
         <v>0</v>
       </c>
       <c r="D444" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E444" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F444" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.3">
@@ -9371,13 +9371,13 @@
         <v>0</v>
       </c>
       <c r="D445" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E445" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F445" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.3">
@@ -9391,13 +9391,13 @@
         <v>0</v>
       </c>
       <c r="D446" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E446" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F446" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="447" spans="1:6" x14ac:dyDescent="0.3">
@@ -9411,13 +9411,13 @@
         <v>0</v>
       </c>
       <c r="D447" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E447" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F447" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="448" spans="1:6" x14ac:dyDescent="0.3">
@@ -9431,13 +9431,13 @@
         <v>0</v>
       </c>
       <c r="D448" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E448" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F448" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="449" spans="1:6" x14ac:dyDescent="0.3">
@@ -9451,13 +9451,13 @@
         <v>0</v>
       </c>
       <c r="D449" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E449" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F449" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="450" spans="1:6" x14ac:dyDescent="0.3">
@@ -9471,13 +9471,13 @@
         <v>1</v>
       </c>
       <c r="D450" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E450" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F450" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="451" spans="1:6" x14ac:dyDescent="0.3">
@@ -9491,13 +9491,13 @@
         <v>0</v>
       </c>
       <c r="D451" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E451" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F451" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.3">
@@ -9511,13 +9511,13 @@
         <v>0</v>
       </c>
       <c r="D452" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E452" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F452" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.3">
@@ -9531,13 +9531,13 @@
         <v>0</v>
       </c>
       <c r="D453" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E453" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F453" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.3">
@@ -9551,13 +9551,13 @@
         <v>0</v>
       </c>
       <c r="D454" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E454" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F454" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.3">
@@ -9571,13 +9571,13 @@
         <v>0</v>
       </c>
       <c r="D455" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E455" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F455" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.3">
@@ -9591,13 +9591,13 @@
         <v>0</v>
       </c>
       <c r="D456" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E456" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F456" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.3">
@@ -9611,13 +9611,13 @@
         <v>0</v>
       </c>
       <c r="D457" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E457" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F457" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.3">
@@ -9631,13 +9631,13 @@
         <v>0.5</v>
       </c>
       <c r="D458" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E458" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F458" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.3">
@@ -9651,13 +9651,13 @@
         <v>0</v>
       </c>
       <c r="D459" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E459" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F459" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.3">
@@ -10091,13 +10091,13 @@
         <v>0</v>
       </c>
       <c r="D481" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E481" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F481" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.3">
@@ -10111,13 +10111,13 @@
         <v>0</v>
       </c>
       <c r="D482" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E482" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F482" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.3">
@@ -10131,13 +10131,13 @@
         <v>0</v>
       </c>
       <c r="D483" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E483" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F483" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.3">
@@ -10151,13 +10151,13 @@
         <v>0</v>
       </c>
       <c r="D484" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E484" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F484" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.3">
@@ -10171,13 +10171,13 @@
         <v>0</v>
       </c>
       <c r="D485" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E485" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F485" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.3">
@@ -10191,13 +10191,13 @@
         <v>0</v>
       </c>
       <c r="D486" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E486" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F486" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.3">
@@ -10211,13 +10211,13 @@
         <v>0</v>
       </c>
       <c r="D487" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E487" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F487" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.3">
@@ -10231,13 +10231,13 @@
         <v>0</v>
       </c>
       <c r="D488" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E488" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F488" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="489" spans="1:6" x14ac:dyDescent="0.3">
@@ -10251,13 +10251,13 @@
         <v>0.5</v>
       </c>
       <c r="D489" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E489" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F489" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.3">
@@ -10271,13 +10271,13 @@
         <v>0</v>
       </c>
       <c r="D490" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E490" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F490" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.3">
@@ -10291,13 +10291,13 @@
         <v>0</v>
       </c>
       <c r="D491" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E491" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F491" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="492" spans="1:6" x14ac:dyDescent="0.3">
@@ -10311,13 +10311,13 @@
         <v>0</v>
       </c>
       <c r="D492" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E492" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F492" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.3">
@@ -10331,13 +10331,13 @@
         <v>0</v>
       </c>
       <c r="D493" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E493" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F493" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="494" spans="1:6" x14ac:dyDescent="0.3">
@@ -10351,13 +10351,13 @@
         <v>0</v>
       </c>
       <c r="D494" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E494" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F494" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="495" spans="1:6" x14ac:dyDescent="0.3">
@@ -10371,13 +10371,13 @@
         <v>0</v>
       </c>
       <c r="D495" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E495" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F495" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="496" spans="1:6" x14ac:dyDescent="0.3">
@@ -10391,13 +10391,13 @@
         <v>0</v>
       </c>
       <c r="D496" s="3">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="E496" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F496" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.3">
@@ -10411,13 +10411,13 @@
         <v>0</v>
       </c>
       <c r="D497" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E497" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F497" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="498" spans="1:6" x14ac:dyDescent="0.3">
@@ -10431,13 +10431,13 @@
         <v>0.5</v>
       </c>
       <c r="D498" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E498" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F498" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.3">
@@ -10451,13 +10451,13 @@
         <v>0</v>
       </c>
       <c r="D499" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E499" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F499" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.3">
@@ -10471,13 +10471,13 @@
         <v>0.5</v>
       </c>
       <c r="D500" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E500" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F500" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.3">
@@ -10491,13 +10491,13 @@
         <v>0</v>
       </c>
       <c r="D501" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E501" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F501" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.3">
@@ -10511,13 +10511,13 @@
         <v>0</v>
       </c>
       <c r="D502" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E502" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F502" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="503" spans="1:6" x14ac:dyDescent="0.3">
@@ -10531,13 +10531,13 @@
         <v>0</v>
       </c>
       <c r="D503" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E503" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F503" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.3">
@@ -10551,13 +10551,13 @@
         <v>0</v>
       </c>
       <c r="D504" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E504" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F504" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.3">
@@ -10571,13 +10571,13 @@
         <v>0</v>
       </c>
       <c r="D505" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E505" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F505" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.3">
@@ -10591,13 +10591,13 @@
         <v>0</v>
       </c>
       <c r="D506" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E506" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F506" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="507" spans="1:6" x14ac:dyDescent="0.3">
@@ -10611,13 +10611,13 @@
         <v>0</v>
       </c>
       <c r="D507" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E507" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F507" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.3">
@@ -10631,13 +10631,13 @@
         <v>0</v>
       </c>
       <c r="D508" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E508" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F508" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.3">
@@ -10651,13 +10651,13 @@
         <v>0</v>
       </c>
       <c r="D509" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E509" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F509" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.3">
@@ -10671,13 +10671,13 @@
         <v>1.5</v>
       </c>
       <c r="D510" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E510" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F510" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.3">
@@ -10691,13 +10691,13 @@
         <v>2.5</v>
       </c>
       <c r="D511" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E511" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F511" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.3">
@@ -10711,13 +10711,13 @@
         <v>1</v>
       </c>
       <c r="D512" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E512" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F512" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="513" spans="1:6" x14ac:dyDescent="0.3">
@@ -10731,13 +10731,13 @@
         <v>0</v>
       </c>
       <c r="D513" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E513" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F513" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="514" spans="1:6" x14ac:dyDescent="0.3">
@@ -10751,13 +10751,13 @@
         <v>0</v>
       </c>
       <c r="D514" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E514" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F514" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="515" spans="1:6" x14ac:dyDescent="0.3">
@@ -10771,13 +10771,13 @@
         <v>0</v>
       </c>
       <c r="D515" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E515" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F515" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.3">
@@ -10791,13 +10791,13 @@
         <v>0</v>
       </c>
       <c r="D516" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E516" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F516" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.3">
@@ -10811,13 +10811,13 @@
         <v>0</v>
       </c>
       <c r="D517" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E517" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F517" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="518" spans="1:6" x14ac:dyDescent="0.3">
@@ -10831,13 +10831,13 @@
         <v>0</v>
       </c>
       <c r="D518" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E518" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F518" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="519" spans="1:6" x14ac:dyDescent="0.3">
@@ -12448,13 +12448,13 @@
         <v>0</v>
       </c>
       <c r="C599" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D599" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E599" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F599" s="3">
         <v>0</v>
@@ -12468,13 +12468,13 @@
         <v>0</v>
       </c>
       <c r="C600" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D600" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E600" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F600" s="3">
         <v>0</v>
@@ -12488,13 +12488,13 @@
         <v>0</v>
       </c>
       <c r="C601" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D601" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E601" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F601" s="3">
         <v>0</v>
@@ -12508,13 +12508,13 @@
         <v>0</v>
       </c>
       <c r="C602" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D602" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E602" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F602" s="3">
         <v>0</v>
@@ -12528,13 +12528,13 @@
         <v>0</v>
       </c>
       <c r="C603" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D603" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E603" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F603" s="3">
         <v>0</v>
@@ -12548,13 +12548,13 @@
         <v>0</v>
       </c>
       <c r="C604" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D604" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E604" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F604" s="3">
         <v>0</v>
@@ -12568,16 +12568,16 @@
         <v>0</v>
       </c>
       <c r="C605" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D605" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E605" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F605" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="606" spans="1:6" x14ac:dyDescent="0.3">
@@ -12588,16 +12588,16 @@
         <v>0</v>
       </c>
       <c r="C606" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D606" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E606" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F606" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="607" spans="1:6" x14ac:dyDescent="0.3">
@@ -12608,16 +12608,16 @@
         <v>0</v>
       </c>
       <c r="C607" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D607" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E607" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F607" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="608" spans="1:6" x14ac:dyDescent="0.3">
@@ -12628,16 +12628,16 @@
         <v>0</v>
       </c>
       <c r="C608" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D608" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E608" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F608" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.3">
@@ -12648,16 +12648,16 @@
         <v>0</v>
       </c>
       <c r="C609" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D609" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E609" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F609" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.3">
@@ -12668,16 +12668,16 @@
         <v>0</v>
       </c>
       <c r="C610" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D610" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E610" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F610" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="611" spans="1:6" x14ac:dyDescent="0.3">
@@ -12688,16 +12688,16 @@
         <v>0</v>
       </c>
       <c r="C611" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D611" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E611" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F611" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.3">
@@ -12708,16 +12708,16 @@
         <v>0</v>
       </c>
       <c r="C612" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D612" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E612" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F612" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.3">
@@ -12728,16 +12728,16 @@
         <v>0</v>
       </c>
       <c r="C613" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D613" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E613" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F613" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.3">
@@ -12748,16 +12748,16 @@
         <v>0</v>
       </c>
       <c r="C614" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D614" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E614" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F614" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="615" spans="1:6" x14ac:dyDescent="0.3">
@@ -12768,16 +12768,16 @@
         <v>0</v>
       </c>
       <c r="C615" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D615" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E615" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F615" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.3">
@@ -12788,16 +12788,16 @@
         <v>0</v>
       </c>
       <c r="C616" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D616" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E616" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F616" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="617" spans="1:6" x14ac:dyDescent="0.3">
@@ -12808,16 +12808,16 @@
         <v>0</v>
       </c>
       <c r="C617" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D617" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E617" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F617" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="618" spans="1:6" x14ac:dyDescent="0.3">
@@ -12828,16 +12828,16 @@
         <v>0</v>
       </c>
       <c r="C618" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D618" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E618" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F618" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="619" spans="1:6" x14ac:dyDescent="0.3">
@@ -12848,16 +12848,16 @@
         <v>0</v>
       </c>
       <c r="C619" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D619" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E619" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F619" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="620" spans="1:6" x14ac:dyDescent="0.3">
@@ -12868,16 +12868,16 @@
         <v>0</v>
       </c>
       <c r="C620" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D620" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E620" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F620" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="621" spans="1:6" x14ac:dyDescent="0.3">
@@ -12888,16 +12888,16 @@
         <v>0</v>
       </c>
       <c r="C621" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D621" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E621" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F621" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="622" spans="1:6" x14ac:dyDescent="0.3">
@@ -12908,16 +12908,16 @@
         <v>0</v>
       </c>
       <c r="C622" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D622" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E622" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F622" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="623" spans="1:6" x14ac:dyDescent="0.3">
@@ -12928,16 +12928,16 @@
         <v>0</v>
       </c>
       <c r="C623" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D623" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E623" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F623" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.3">
@@ -12948,16 +12948,16 @@
         <v>0</v>
       </c>
       <c r="C624" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D624" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E624" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F624" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.3">
@@ -12968,16 +12968,16 @@
         <v>0</v>
       </c>
       <c r="C625" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D625" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E625" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F625" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="626" spans="1:6" x14ac:dyDescent="0.3">
@@ -12988,16 +12988,16 @@
         <v>0</v>
       </c>
       <c r="C626" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D626" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E626" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F626" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="627" spans="1:6" x14ac:dyDescent="0.3">
@@ -13008,16 +13008,16 @@
         <v>0</v>
       </c>
       <c r="C627" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D627" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E627" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F627" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="628" spans="1:6" x14ac:dyDescent="0.3">
@@ -13028,16 +13028,16 @@
         <v>0</v>
       </c>
       <c r="C628" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D628" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E628" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F628" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.3">
@@ -13048,16 +13048,16 @@
         <v>0</v>
       </c>
       <c r="C629" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D629" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E629" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F629" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.3">
@@ -13068,16 +13068,16 @@
         <v>0</v>
       </c>
       <c r="C630" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D630" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E630" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F630" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="631" spans="1:6" x14ac:dyDescent="0.3">
@@ -13088,16 +13088,16 @@
         <v>0</v>
       </c>
       <c r="C631" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D631" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E631" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F631" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="632" spans="1:6" x14ac:dyDescent="0.3">
@@ -13108,16 +13108,16 @@
         <v>0</v>
       </c>
       <c r="C632" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D632" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E632" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F632" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="633" spans="1:6" x14ac:dyDescent="0.3">
@@ -13128,16 +13128,16 @@
         <v>0</v>
       </c>
       <c r="C633" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D633" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E633" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F633" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.3">
@@ -13148,16 +13148,16 @@
         <v>0</v>
       </c>
       <c r="C634" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D634" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E634" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F634" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="635" spans="1:6" x14ac:dyDescent="0.3">
@@ -13168,16 +13168,16 @@
         <v>0</v>
       </c>
       <c r="C635" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D635" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E635" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F635" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="636" spans="1:6" x14ac:dyDescent="0.3">
@@ -13188,16 +13188,16 @@
         <v>0</v>
       </c>
       <c r="C636" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D636" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E636" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F636" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.3">
@@ -13208,16 +13208,16 @@
         <v>0</v>
       </c>
       <c r="C637" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D637" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E637" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F637" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.3">
@@ -13228,16 +13228,16 @@
         <v>0</v>
       </c>
       <c r="C638" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D638" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E638" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F638" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.3">
@@ -13248,16 +13248,16 @@
         <v>0</v>
       </c>
       <c r="C639" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D639" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E639" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F639" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.3">
@@ -13268,16 +13268,16 @@
         <v>0</v>
       </c>
       <c r="C640" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D640" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E640" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F640" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="641" spans="1:6" x14ac:dyDescent="0.3">
@@ -13288,16 +13288,16 @@
         <v>0</v>
       </c>
       <c r="C641" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D641" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E641" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F641" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="642" spans="1:6" x14ac:dyDescent="0.3">
@@ -13308,16 +13308,16 @@
         <v>0</v>
       </c>
       <c r="C642" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D642" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E642" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F642" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="643" spans="1:6" x14ac:dyDescent="0.3">
@@ -13328,13 +13328,13 @@
         <v>0</v>
       </c>
       <c r="C643" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D643" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E643" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F643" s="3">
         <v>0</v>
@@ -13348,13 +13348,13 @@
         <v>0</v>
       </c>
       <c r="C644" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D644" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E644" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F644" s="3">
         <v>0</v>
@@ -13368,13 +13368,13 @@
         <v>0</v>
       </c>
       <c r="C645" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D645" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E645" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F645" s="3">
         <v>0</v>
@@ -13388,13 +13388,13 @@
         <v>0</v>
       </c>
       <c r="C646" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D646" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E646" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F646" s="3">
         <v>0</v>
@@ -13408,13 +13408,13 @@
         <v>0</v>
       </c>
       <c r="C647" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D647" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E647" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F647" s="3">
         <v>0</v>
@@ -13428,13 +13428,13 @@
         <v>0</v>
       </c>
       <c r="C648" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D648" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E648" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F648" s="3">
         <v>0.5</v>
@@ -13448,13 +13448,13 @@
         <v>0</v>
       </c>
       <c r="C649" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D649" s="3">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="E649" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F649" s="3">
         <v>0</v>
@@ -13468,13 +13468,13 @@
         <v>0</v>
       </c>
       <c r="C650" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D650" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E650" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F650" s="3">
         <v>0</v>
@@ -13488,13 +13488,13 @@
         <v>0</v>
       </c>
       <c r="C651" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D651" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E651" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F651" s="3">
         <v>0</v>
@@ -13508,13 +13508,13 @@
         <v>0</v>
       </c>
       <c r="C652" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D652" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E652" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F652" s="3">
         <v>0</v>
@@ -13528,13 +13528,13 @@
         <v>0</v>
       </c>
       <c r="C653" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D653" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E653" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F653" s="3">
         <v>0</v>
@@ -13548,13 +13548,13 @@
         <v>0</v>
       </c>
       <c r="C654" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D654" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E654" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F654" s="3">
         <v>0</v>
@@ -13568,13 +13568,13 @@
         <v>0</v>
       </c>
       <c r="C655" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D655" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E655" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F655" s="3">
         <v>0</v>
@@ -13588,13 +13588,13 @@
         <v>0</v>
       </c>
       <c r="C656" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D656" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E656" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F656" s="3">
         <v>0</v>
@@ -13608,13 +13608,13 @@
         <v>0.5</v>
       </c>
       <c r="C657" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D657" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E657" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F657" s="3">
         <v>0</v>
@@ -13628,13 +13628,13 @@
         <v>0</v>
       </c>
       <c r="C658" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D658" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E658" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F658" s="3">
         <v>0</v>
@@ -13648,13 +13648,13 @@
         <v>0</v>
       </c>
       <c r="C659" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D659" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E659" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F659" s="3">
         <v>0</v>
@@ -13668,13 +13668,13 @@
         <v>0</v>
       </c>
       <c r="C660" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D660" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E660" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F660" s="3">
         <v>0</v>
@@ -13688,13 +13688,13 @@
         <v>0</v>
       </c>
       <c r="C661" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D661" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E661" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F661" s="3">
         <v>0</v>
@@ -13708,13 +13708,13 @@
         <v>0</v>
       </c>
       <c r="C662" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D662" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E662" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F662" s="3">
         <v>0</v>
@@ -13728,13 +13728,13 @@
         <v>0</v>
       </c>
       <c r="C663" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D663" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E663" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F663" s="3">
         <v>0</v>
@@ -13748,13 +13748,13 @@
         <v>0</v>
       </c>
       <c r="C664" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D664" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E664" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F664" s="3">
         <v>0</v>
@@ -13768,13 +13768,13 @@
         <v>0</v>
       </c>
       <c r="C665" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D665" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E665" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F665" s="3">
         <v>0</v>
@@ -13788,13 +13788,13 @@
         <v>0</v>
       </c>
       <c r="C666" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D666" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E666" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F666" s="3">
         <v>0</v>
@@ -13808,13 +13808,13 @@
         <v>0</v>
       </c>
       <c r="C667" s="3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D667" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E667" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F667" s="3">
         <v>0.5</v>
@@ -13828,13 +13828,13 @@
         <v>0</v>
       </c>
       <c r="C668" s="3">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D668" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E668" s="3">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="F668" s="3">
         <v>2.5</v>
@@ -13848,13 +13848,13 @@
         <v>11</v>
       </c>
       <c r="C669" s="3">
-        <v>24.5</v>
+        <v>3</v>
       </c>
       <c r="D669" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E669" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F669" s="3">
         <v>26.5</v>
@@ -13868,13 +13868,13 @@
         <v>4</v>
       </c>
       <c r="C670" s="3">
-        <v>12.5</v>
+        <v>3</v>
       </c>
       <c r="D670" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E670" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F670" s="3">
         <v>3.5</v>
@@ -13888,10 +13888,10 @@
         <v>3</v>
       </c>
       <c r="C671" s="3">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="D671" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E671" s="3">
         <v>3</v>
@@ -13908,10 +13908,10 @@
         <v>1</v>
       </c>
       <c r="C672" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D672" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E672" s="3">
         <v>3</v>
@@ -13928,13 +13928,13 @@
         <v>2</v>
       </c>
       <c r="C673" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D673" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E673" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F673" s="3">
         <v>0</v>
@@ -13948,13 +13948,13 @@
         <v>0</v>
       </c>
       <c r="C674" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D674" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E674" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F674" s="3">
         <v>1</v>

</xml_diff>